<commit_message>
training monitoring is update
</commit_message>
<xml_diff>
--- a/training_monitoring.xlsx
+++ b/training_monitoring.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="34">
   <si>
     <t>bs</t>
   </si>
@@ -97,19 +97,25 @@
     <t>500k</t>
   </si>
   <si>
-    <t>mixup with prob 5</t>
-  </si>
-  <si>
     <t>augmentation on all data</t>
   </si>
   <si>
     <t>_v5</t>
   </si>
   <si>
-    <t>all  aug</t>
-  </si>
-  <si>
-    <t>10,000k</t>
+    <t>24,000k</t>
+  </si>
+  <si>
+    <t>mixup with prob 3/4</t>
+  </si>
+  <si>
+    <t>mixup with prob 1</t>
+  </si>
+  <si>
+    <t>with focal</t>
+  </si>
+  <si>
+    <t>prob 1</t>
   </si>
 </sst>
 </file>
@@ -258,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,10 +293,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -299,10 +308,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1276,16 +1291,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>475805</xdr:colOff>
-      <xdr:row>239</xdr:row>
-      <xdr:rowOff>152104</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>180530</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>37804</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1302,8 +1317,198 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6629400" y="43643550"/>
+          <a:off x="5724525" y="43719750"/>
           <a:ext cx="3561905" cy="2371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>799658</xdr:colOff>
+      <xdr:row>256</xdr:row>
+      <xdr:rowOff>161620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="46843950"/>
+          <a:ext cx="3533333" cy="2438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>258</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>113857</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>66368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="49606200"/>
+          <a:ext cx="3542857" cy="2457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>273</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>256734</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>113994</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="962025" y="52539900"/>
+          <a:ext cx="3523809" cy="2447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>273</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>371039</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>199711</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4772025" y="52558950"/>
+          <a:ext cx="3485714" cy="2514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>288</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409137</xdr:colOff>
+      <xdr:row>300</xdr:row>
+      <xdr:rowOff>142589</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="55416450"/>
+          <a:ext cx="3504762" cy="2285714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1602,10 +1807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W243"/>
+  <dimension ref="A1:W289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="K247" sqref="K247"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="K293" sqref="K293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,11 +2038,11 @@
       <c r="G103" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H103" s="10" t="s">
+      <c r="H103" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I103" s="10"/>
-      <c r="J103" s="10"/>
+      <c r="I103" s="12"/>
+      <c r="J103" s="12"/>
     </row>
     <row r="115" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1860,15 +2065,15 @@
       <c r="G116" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H116" s="12" t="s">
+      <c r="H116" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I116" s="12"/>
-      <c r="J116" s="12"/>
-      <c r="K116" s="12" t="s">
+      <c r="I116" s="13"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="L116" s="12"/>
+      <c r="L116" s="13"/>
     </row>
     <row r="128" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1891,15 +2096,15 @@
       <c r="G129" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H129" s="10" t="s">
+      <c r="H129" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I129" s="10"/>
-      <c r="J129" s="10"/>
-      <c r="K129" s="10" t="s">
+      <c r="I129" s="12"/>
+      <c r="J129" s="12"/>
+      <c r="K129" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L129" s="10"/>
+      <c r="L129" s="12"/>
       <c r="N129" s="4" t="s">
         <v>13</v>
       </c>
@@ -1925,22 +2130,22 @@
       <c r="G143" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H143" s="10" t="s">
+      <c r="H143" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I143" s="10"/>
-      <c r="J143" s="10"/>
-      <c r="K143" s="10" t="s">
+      <c r="I143" s="12"/>
+      <c r="J143" s="12"/>
+      <c r="K143" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L143" s="10"/>
+      <c r="L143" s="12"/>
       <c r="N143" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P143" s="10" t="s">
+      <c r="P143" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Q143" s="10"/>
+      <c r="Q143" s="12"/>
     </row>
     <row r="155" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="156" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1963,22 +2168,22 @@
       <c r="G156" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H156" s="10" t="s">
+      <c r="H156" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I156" s="10"/>
-      <c r="J156" s="10"/>
-      <c r="K156" s="10" t="s">
+      <c r="I156" s="12"/>
+      <c r="J156" s="12"/>
+      <c r="K156" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L156" s="10"/>
+      <c r="L156" s="12"/>
       <c r="N156" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P156" s="11" t="s">
+      <c r="P156" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="Q156" s="11"/>
+      <c r="Q156" s="18"/>
     </row>
     <row r="168" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="169" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2001,20 +2206,20 @@
       <c r="G169" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H169" s="10" t="s">
+      <c r="H169" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I169" s="10"/>
-      <c r="J169" s="10"/>
-      <c r="K169" s="10" t="s">
+      <c r="I169" s="12"/>
+      <c r="J169" s="12"/>
+      <c r="K169" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L169" s="10"/>
+      <c r="L169" s="12"/>
       <c r="N169" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P169" s="11"/>
-      <c r="Q169" s="11"/>
+      <c r="P169" s="18"/>
+      <c r="Q169" s="18"/>
     </row>
     <row r="180" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="181" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2039,18 +2244,18 @@
       <c r="G181" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H181" s="10" t="s">
+      <c r="H181" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I181" s="10"/>
-      <c r="J181" s="10"/>
-      <c r="K181" s="10"/>
-      <c r="L181" s="10"/>
+      <c r="I181" s="12"/>
+      <c r="J181" s="12"/>
+      <c r="K181" s="12"/>
+      <c r="L181" s="12"/>
       <c r="N181" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P181" s="11"/>
-      <c r="Q181" s="11"/>
+      <c r="P181" s="18"/>
+      <c r="Q181" s="18"/>
     </row>
     <row r="195" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="196" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2075,19 +2280,19 @@
       <c r="G196" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H196" s="10" t="s">
+      <c r="H196" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I196" s="10"/>
-      <c r="J196" s="10"/>
-      <c r="K196" s="10"/>
-      <c r="L196" s="10"/>
-      <c r="M196" s="10" t="s">
+      <c r="I196" s="12"/>
+      <c r="J196" s="12"/>
+      <c r="K196" s="12"/>
+      <c r="L196" s="12"/>
+      <c r="M196" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N196" s="10"/>
-      <c r="P196" s="11"/>
-      <c r="Q196" s="11"/>
+      <c r="N196" s="12"/>
+      <c r="P196" s="18"/>
+      <c r="Q196" s="18"/>
     </row>
     <row r="210" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="211" spans="1:18" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2112,21 +2317,21 @@
       <c r="G211" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H211" s="10" t="s">
+      <c r="H211" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I211" s="10"/>
-      <c r="J211" s="10"/>
-      <c r="K211" s="10" t="s">
+      <c r="I211" s="12"/>
+      <c r="J211" s="12"/>
+      <c r="K211" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L211" s="10"/>
-      <c r="M211" s="10"/>
-      <c r="N211" s="10"/>
-      <c r="O211" s="10"/>
-      <c r="P211" s="10"/>
-      <c r="Q211" s="10"/>
-      <c r="R211" s="10"/>
+      <c r="L211" s="12"/>
+      <c r="M211" s="12"/>
+      <c r="N211" s="12"/>
+      <c r="O211" s="12"/>
+      <c r="P211" s="12"/>
+      <c r="Q211" s="12"/>
+      <c r="R211" s="12"/>
     </row>
     <row r="225" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="226" spans="1:23" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2151,47 +2356,53 @@
       <c r="G226" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H226" s="12" t="s">
+      <c r="H226" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I226" s="12"/>
-      <c r="J226" s="12"/>
-      <c r="K226" s="12" t="s">
+      <c r="I226" s="13"/>
+      <c r="J226" s="13"/>
+      <c r="K226" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L226" s="12"/>
-      <c r="M226" s="12"/>
-      <c r="N226" s="12"/>
-      <c r="O226" s="12" t="s">
+      <c r="L226" s="13"/>
+      <c r="M226" s="13"/>
+      <c r="N226" s="13"/>
+      <c r="O226" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="P226" s="12"/>
-      <c r="Q226" s="12"/>
-      <c r="R226" s="12"/>
-      <c r="S226" s="12" t="s">
+      <c r="P226" s="13"/>
+      <c r="Q226" s="13"/>
+      <c r="R226" s="13"/>
+      <c r="S226" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="T226" s="14"/>
+      <c r="U226" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="T226" s="13"/>
-      <c r="U226" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="V226" s="10"/>
-      <c r="W226" s="10"/>
+      <c r="V226" s="12"/>
+      <c r="W226" s="12"/>
     </row>
     <row r="227" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C227" s="1">
+        <v>128</v>
+      </c>
       <c r="H227" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I227" s="15"/>
       <c r="J227" s="15"/>
-    </row>
-    <row r="242" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="243" spans="1:21" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T227" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="242" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="243" spans="1:23" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B243" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="B243" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="C243" s="9">
         <v>128</v>
@@ -2206,41 +2417,225 @@
         <v>6</v>
       </c>
       <c r="G243" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H243" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I243" s="13"/>
+      <c r="J243" s="13"/>
+      <c r="K243" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L243" s="13"/>
+      <c r="M243" s="13"/>
+      <c r="N243" s="13"/>
+      <c r="O243" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P243" s="13"/>
+      <c r="Q243" s="13"/>
+      <c r="R243" s="13"/>
+      <c r="S243" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H243" s="12" t="s">
+      <c r="T243" s="17"/>
+      <c r="U243" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V243" s="12"/>
+      <c r="W243" s="12"/>
+    </row>
+    <row r="244" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H244" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I244" s="15"/>
+      <c r="J244" s="15"/>
+    </row>
+    <row r="257" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="258" spans="1:23" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B258" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C258" s="9">
+        <v>128</v>
+      </c>
+      <c r="D258" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E258" s="9">
+        <v>128</v>
+      </c>
+      <c r="F258" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G258" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H258" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I243" s="12"/>
-      <c r="J243" s="12"/>
-      <c r="K243" s="12" t="s">
+      <c r="I258" s="13"/>
+      <c r="J258" s="13"/>
+      <c r="K258" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L243" s="12"/>
-      <c r="M243" s="12"/>
-      <c r="N243" s="12"/>
-      <c r="O243" s="12" t="s">
+      <c r="L258" s="13"/>
+      <c r="M258" s="13"/>
+      <c r="N258" s="13"/>
+      <c r="O258" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="P243" s="12"/>
-      <c r="Q243" s="12"/>
-      <c r="R243" s="12"/>
-      <c r="S243" s="14" t="s">
+      <c r="P258" s="13"/>
+      <c r="Q258" s="13"/>
+      <c r="R258" s="13"/>
+      <c r="S258" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="T258" s="17"/>
+      <c r="U258" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V258" s="12"/>
+      <c r="W258" s="12"/>
+    </row>
+    <row r="259" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H259" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I259" s="15"/>
+      <c r="J259" s="15"/>
+    </row>
+    <row r="272" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="273" spans="1:23" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A273" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="T243" s="10"/>
-      <c r="U243" s="10"/>
+      <c r="B273" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C273" s="9">
+        <v>128</v>
+      </c>
+      <c r="D273" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E273" s="9">
+        <v>128</v>
+      </c>
+      <c r="F273" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G273" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H273" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I273" s="13"/>
+      <c r="J273" s="13"/>
+      <c r="K273" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L273" s="13"/>
+      <c r="M273" s="13"/>
+      <c r="N273" s="13"/>
+      <c r="O273" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P273" s="13"/>
+      <c r="Q273" s="13"/>
+      <c r="R273" s="13"/>
+      <c r="S273" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T273" s="14"/>
+      <c r="U273" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V273" s="12"/>
+      <c r="W273" s="12"/>
+    </row>
+    <row r="274" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H274" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I274" s="10"/>
+      <c r="J274" s="10"/>
+    </row>
+    <row r="287" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="288" spans="1:23" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B288" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C288" s="9">
+        <v>128</v>
+      </c>
+      <c r="D288" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="E288" s="9">
+        <v>128</v>
+      </c>
+      <c r="F288" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G288" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H288" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I288" s="13"/>
+      <c r="J288" s="13"/>
+      <c r="K288" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L288" s="13"/>
+      <c r="M288" s="13"/>
+      <c r="N288" s="13"/>
+      <c r="O288" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P288" s="13"/>
+      <c r="Q288" s="13"/>
+      <c r="R288" s="13"/>
+      <c r="S288" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="T288" s="14"/>
+      <c r="U288" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V288" s="12"/>
+      <c r="W288" s="12"/>
+    </row>
+    <row r="289" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H289" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I289" s="10"/>
+      <c r="J289" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="S243:U243"/>
-    <mergeCell ref="H227:J227"/>
-    <mergeCell ref="H243:J243"/>
-    <mergeCell ref="K243:N243"/>
-    <mergeCell ref="O243:R243"/>
-    <mergeCell ref="H226:J226"/>
-    <mergeCell ref="K226:N226"/>
-    <mergeCell ref="O226:R226"/>
+  <mergeCells count="54">
+    <mergeCell ref="H211:J211"/>
+    <mergeCell ref="K211:N211"/>
+    <mergeCell ref="H181:J181"/>
+    <mergeCell ref="K181:L181"/>
+    <mergeCell ref="P181:Q181"/>
+    <mergeCell ref="H196:J196"/>
+    <mergeCell ref="K196:L196"/>
+    <mergeCell ref="P196:Q196"/>
+    <mergeCell ref="M196:N196"/>
+    <mergeCell ref="O211:R211"/>
     <mergeCell ref="S226:T226"/>
     <mergeCell ref="U226:W226"/>
     <mergeCell ref="H103:J103"/>
@@ -2257,16 +2652,34 @@
     <mergeCell ref="P169:Q169"/>
     <mergeCell ref="H143:J143"/>
     <mergeCell ref="K143:L143"/>
-    <mergeCell ref="H211:J211"/>
-    <mergeCell ref="K211:N211"/>
-    <mergeCell ref="H181:J181"/>
-    <mergeCell ref="K181:L181"/>
-    <mergeCell ref="P181:Q181"/>
-    <mergeCell ref="H196:J196"/>
-    <mergeCell ref="K196:L196"/>
-    <mergeCell ref="P196:Q196"/>
-    <mergeCell ref="M196:N196"/>
-    <mergeCell ref="O211:R211"/>
+    <mergeCell ref="H227:J227"/>
+    <mergeCell ref="H243:J243"/>
+    <mergeCell ref="K243:N243"/>
+    <mergeCell ref="O243:R243"/>
+    <mergeCell ref="H226:J226"/>
+    <mergeCell ref="K226:N226"/>
+    <mergeCell ref="O226:R226"/>
+    <mergeCell ref="S243:T243"/>
+    <mergeCell ref="U243:W243"/>
+    <mergeCell ref="H244:J244"/>
+    <mergeCell ref="H258:J258"/>
+    <mergeCell ref="K258:N258"/>
+    <mergeCell ref="O258:R258"/>
+    <mergeCell ref="S258:T258"/>
+    <mergeCell ref="U258:W258"/>
+    <mergeCell ref="H259:J259"/>
+    <mergeCell ref="H273:J273"/>
+    <mergeCell ref="K273:N273"/>
+    <mergeCell ref="O273:R273"/>
+    <mergeCell ref="S273:T273"/>
+    <mergeCell ref="H289:J289"/>
+    <mergeCell ref="U273:W273"/>
+    <mergeCell ref="H274:J274"/>
+    <mergeCell ref="H288:J288"/>
+    <mergeCell ref="K288:N288"/>
+    <mergeCell ref="O288:R288"/>
+    <mergeCell ref="S288:T288"/>
+    <mergeCell ref="U288:W288"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>